<commit_message>
Edgecomparison works but not optimized. Next up: optimize GetTexture that now allocates memory.
</commit_message>
<xml_diff>
--- a/WorldParser/World.xlsx
+++ b/WorldParser/World.xlsx
@@ -132,7 +132,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -162,10 +162,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -252,13 +248,13 @@
   </sheetPr>
   <dimension ref="A1:EY103"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="CU31" activeCellId="0" sqref="CU31"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="2.39285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="2.29591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1891,6 +1887,10 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
       <c r="AL14" s="4"/>
       <c r="AM14" s="4"/>
       <c r="AN14" s="4"/>
@@ -1971,6 +1971,10 @@
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4"/>
       <c r="AK15" s="4"/>
       <c r="AL15" s="4"/>
       <c r="AM15" s="4"/>
@@ -2059,22 +2063,10 @@
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
       <c r="S16" s="4"/>
-      <c r="T16" s="4"/>
       <c r="U16" s="4"/>
       <c r="V16" s="4"/>
       <c r="W16" s="4"/>
-      <c r="X16" s="4"/>
-      <c r="Y16" s="4"/>
-      <c r="Z16" s="4"/>
-      <c r="AA16" s="4"/>
-      <c r="AB16" s="4"/>
-      <c r="AC16" s="4"/>
-      <c r="AD16" s="4"/>
-      <c r="AE16" s="4"/>
       <c r="AF16" s="4"/>
       <c r="AG16" s="4"/>
       <c r="AH16" s="4"/>
@@ -2205,22 +2197,6 @@
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-      <c r="U17" s="4"/>
-      <c r="V17" s="4"/>
-      <c r="W17" s="4"/>
-      <c r="X17" s="4"/>
-      <c r="Y17" s="4"/>
-      <c r="Z17" s="4"/>
-      <c r="AA17" s="4"/>
-      <c r="AB17" s="4"/>
-      <c r="AC17" s="4"/>
-      <c r="AD17" s="4"/>
-      <c r="AE17" s="4"/>
       <c r="AF17" s="4"/>
       <c r="AG17" s="4"/>
       <c r="AH17" s="4"/>
@@ -2326,21 +2302,10 @@
     </row>
     <row r="18" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="R18" s="4"/>
       <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
       <c r="U18" s="4"/>
       <c r="V18" s="4"/>
       <c r="W18" s="4"/>
-      <c r="X18" s="4"/>
-      <c r="Y18" s="4"/>
-      <c r="Z18" s="4"/>
-      <c r="AA18" s="4"/>
-      <c r="AB18" s="4"/>
-      <c r="AC18" s="4"/>
-      <c r="AD18" s="4"/>
-      <c r="AE18" s="4"/>
       <c r="AF18" s="4"/>
       <c r="AG18" s="4"/>
       <c r="AH18" s="4"/>
@@ -2439,20 +2404,6 @@
     <row r="19" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
-      <c r="U19" s="4"/>
-      <c r="V19" s="4"/>
-      <c r="W19" s="4"/>
-      <c r="X19" s="4"/>
-      <c r="Y19" s="4"/>
-      <c r="Z19" s="4"/>
-      <c r="AA19" s="4"/>
-      <c r="AB19" s="4"/>
-      <c r="AC19" s="4"/>
-      <c r="AD19" s="4"/>
-      <c r="AE19" s="4"/>
       <c r="AF19" s="4"/>
       <c r="AG19" s="4"/>
       <c r="AH19" s="4"/>
@@ -2552,19 +2503,6 @@
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="T20" s="4"/>
-      <c r="U20" s="4"/>
-      <c r="V20" s="4"/>
-      <c r="W20" s="4"/>
-      <c r="X20" s="4"/>
-      <c r="Y20" s="4"/>
-      <c r="Z20" s="4"/>
-      <c r="AA20" s="4"/>
-      <c r="AB20" s="4"/>
-      <c r="AC20" s="4"/>
-      <c r="AD20" s="4"/>
-      <c r="AE20" s="4"/>
       <c r="AF20" s="4"/>
       <c r="AG20" s="4"/>
       <c r="AH20" s="4"/>
@@ -2664,19 +2602,6 @@
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
-      <c r="P21" s="4"/>
-      <c r="T21" s="4"/>
-      <c r="U21" s="4"/>
-      <c r="V21" s="4"/>
-      <c r="W21" s="4"/>
-      <c r="X21" s="4"/>
-      <c r="Y21" s="4"/>
-      <c r="Z21" s="4"/>
-      <c r="AA21" s="4"/>
-      <c r="AB21" s="4"/>
-      <c r="AC21" s="4"/>
-      <c r="AD21" s="4"/>
-      <c r="AE21" s="4"/>
       <c r="AF21" s="4"/>
       <c r="AG21" s="4"/>
       <c r="AH21" s="4"/>
@@ -2777,7 +2702,6 @@
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-      <c r="P22" s="4"/>
       <c r="AH22" s="4"/>
       <c r="AI22" s="4"/>
       <c r="AJ22" s="4"/>
@@ -6004,11 +5928,6 @@
       <c r="BG46" s="7"/>
       <c r="BH46" s="7"/>
       <c r="BI46" s="7"/>
-      <c r="BJ46" s="8"/>
-      <c r="BK46" s="8"/>
-      <c r="BL46" s="8"/>
-      <c r="BM46" s="8"/>
-      <c r="BN46" s="8"/>
       <c r="CL46" s="4"/>
       <c r="CM46" s="4"/>
       <c r="CN46" s="4"/>
@@ -6085,10 +6004,6 @@
       <c r="BH47" s="7"/>
       <c r="BI47" s="7"/>
       <c r="BJ47" s="7"/>
-      <c r="BK47" s="8"/>
-      <c r="BL47" s="8"/>
-      <c r="BM47" s="8"/>
-      <c r="BN47" s="8"/>
       <c r="CK47" s="4"/>
       <c r="CL47" s="4"/>
       <c r="CM47" s="4"/>
@@ -6171,9 +6086,6 @@
       <c r="BI48" s="7"/>
       <c r="BJ48" s="7"/>
       <c r="BK48" s="7"/>
-      <c r="BL48" s="8"/>
-      <c r="BM48" s="8"/>
-      <c r="BN48" s="8"/>
       <c r="CJ48" s="4"/>
       <c r="CK48" s="4"/>
       <c r="CL48" s="4"/>
@@ -6421,17 +6333,6 @@
       <c r="BA50" s="7"/>
       <c r="BB50" s="7"/>
       <c r="BC50" s="7"/>
-      <c r="BD50" s="8"/>
-      <c r="BE50" s="8"/>
-      <c r="BF50" s="8"/>
-      <c r="BG50" s="8"/>
-      <c r="BH50" s="8"/>
-      <c r="BI50" s="8"/>
-      <c r="BJ50" s="8"/>
-      <c r="BK50" s="8"/>
-      <c r="BL50" s="8"/>
-      <c r="BM50" s="8"/>
-      <c r="BN50" s="8"/>
       <c r="BO50" s="4"/>
       <c r="BP50" s="4"/>
       <c r="BQ50" s="4"/>
@@ -6549,20 +6450,6 @@
       <c r="AX51" s="4"/>
       <c r="AY51" s="5"/>
       <c r="AZ51" s="7"/>
-      <c r="BA51" s="8"/>
-      <c r="BB51" s="8"/>
-      <c r="BC51" s="8"/>
-      <c r="BD51" s="8"/>
-      <c r="BE51" s="8"/>
-      <c r="BF51" s="8"/>
-      <c r="BG51" s="8"/>
-      <c r="BH51" s="8"/>
-      <c r="BI51" s="8"/>
-      <c r="BJ51" s="8"/>
-      <c r="BK51" s="8"/>
-      <c r="BL51" s="8"/>
-      <c r="BM51" s="8"/>
-      <c r="BN51" s="8"/>
       <c r="BO51" s="4"/>
       <c r="BQ51" s="4"/>
       <c r="BR51" s="4"/>
@@ -6676,19 +6563,6 @@
       <c r="AY52" s="5"/>
       <c r="AZ52" s="7"/>
       <c r="BA52" s="7"/>
-      <c r="BB52" s="8"/>
-      <c r="BC52" s="8"/>
-      <c r="BD52" s="8"/>
-      <c r="BE52" s="8"/>
-      <c r="BF52" s="8"/>
-      <c r="BG52" s="8"/>
-      <c r="BH52" s="8"/>
-      <c r="BI52" s="8"/>
-      <c r="BJ52" s="8"/>
-      <c r="BK52" s="8"/>
-      <c r="BL52" s="8"/>
-      <c r="BM52" s="8"/>
-      <c r="BN52" s="8"/>
       <c r="BO52" s="4"/>
       <c r="BR52" s="4"/>
       <c r="BS52" s="4"/>
@@ -6802,18 +6676,6 @@
       <c r="AZ53" s="7"/>
       <c r="BA53" s="7"/>
       <c r="BB53" s="7"/>
-      <c r="BC53" s="8"/>
-      <c r="BD53" s="8"/>
-      <c r="BE53" s="8"/>
-      <c r="BF53" s="8"/>
-      <c r="BG53" s="8"/>
-      <c r="BH53" s="8"/>
-      <c r="BI53" s="8"/>
-      <c r="BJ53" s="8"/>
-      <c r="BK53" s="8"/>
-      <c r="BL53" s="8"/>
-      <c r="BM53" s="8"/>
-      <c r="BN53" s="8"/>
       <c r="BO53" s="4"/>
       <c r="BS53" s="4"/>
       <c r="BT53" s="4"/>
@@ -6926,18 +6788,6 @@
       <c r="AZ54" s="7"/>
       <c r="BA54" s="7"/>
       <c r="BB54" s="7"/>
-      <c r="BC54" s="8"/>
-      <c r="BD54" s="8"/>
-      <c r="BE54" s="8"/>
-      <c r="BF54" s="8"/>
-      <c r="BG54" s="8"/>
-      <c r="BH54" s="8"/>
-      <c r="BI54" s="8"/>
-      <c r="BJ54" s="8"/>
-      <c r="BK54" s="8"/>
-      <c r="BL54" s="8"/>
-      <c r="BM54" s="8"/>
-      <c r="BN54" s="8"/>
       <c r="BO54" s="4"/>
       <c r="BS54" s="4"/>
       <c r="BT54" s="4"/>
@@ -7038,17 +6888,6 @@
       <c r="BA55" s="7"/>
       <c r="BB55" s="7"/>
       <c r="BC55" s="7"/>
-      <c r="BD55" s="8"/>
-      <c r="BE55" s="8"/>
-      <c r="BF55" s="8"/>
-      <c r="BG55" s="8"/>
-      <c r="BH55" s="8"/>
-      <c r="BI55" s="8"/>
-      <c r="BJ55" s="8"/>
-      <c r="BK55" s="8"/>
-      <c r="BL55" s="8"/>
-      <c r="BM55" s="8"/>
-      <c r="BN55" s="8"/>
       <c r="BO55" s="4"/>
       <c r="CG55" s="4"/>
       <c r="CH55" s="4"/>
@@ -13486,28 +13325,28 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">

</xml_diff>